<commit_message>
restructure the codebase to 1) reduce code redunduncies 2) enable more options for subcommands
</commit_message>
<xml_diff>
--- a/cmd/cli/testdata/test02.xlsx
+++ b/cmd/cli/testdata/test02.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pyan\github\otlh\cmd\cli\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{257A07C3-A233-4313-A381-3DA201CD1372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76467453-56FE-4733-90FD-8C4F9E4D05B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4290" yWindow="4290" windowWidth="28800" windowHeight="15435" tabRatio="64" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="38700" windowHeight="15435" tabRatio="64" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -111,13 +111,13 @@
     <t>Brent Richardson</t>
   </si>
   <si>
-    <t>Imoprtbrenttest-2</t>
-  </si>
-  <si>
-    <t>Brenttest-2</t>
-  </si>
-  <si>
-    <t>Legal hold test-2</t>
+    <t>Imoprtbrenttest-3</t>
+  </si>
+  <si>
+    <t>Brenttest-3</t>
+  </si>
+  <si>
+    <t>Legal hold test-3</t>
   </si>
 </sst>
 </file>
@@ -840,7 +840,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2266,9 +2266,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2404,19 +2407,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68F4E22A-36AD-4C4E-96D1-0557CECA5953}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48245400-466E-4767-B208-B428FA6F603E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2440,9 +2439,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48245400-466E-4767-B208-B428FA6F603E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68F4E22A-36AD-4C4E-96D1-0557CECA5953}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
silent hold importer feature ready
</commit_message>
<xml_diff>
--- a/cmd/cli/testdata/test02.xlsx
+++ b/cmd/cli/testdata/test02.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pyan\github\otlh\cmd\cli\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76467453-56FE-4733-90FD-8C4F9E4D05B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A718058-8E5D-4776-BA13-B1C86A3DFE54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="38700" windowHeight="15435" tabRatio="64" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9855" yWindow="5340" windowWidth="38700" windowHeight="15435" tabRatio="64" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>DO NOT ALTER THE FORMATTING OF THIS TEMPLATE</t>
   </si>
@@ -99,9 +99,6 @@
     <t>Attachment Names</t>
   </si>
   <si>
-    <t>Legal hold test</t>
-  </si>
-  <si>
     <t>brichardson@opentext.com</t>
   </si>
   <si>
@@ -117,7 +114,13 @@
     <t>Brenttest-3</t>
   </si>
   <si>
-    <t>Legal hold test-3</t>
+    <t>Legal hold test-5</t>
+  </si>
+  <si>
+    <t>Legal hold test-sub5</t>
+  </si>
+  <si>
+    <t>Legal hold test-title5</t>
   </si>
 </sst>
 </file>
@@ -840,7 +843,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -972,25 +975,25 @@
     </row>
     <row r="7" spans="1:12" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="C7" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="D7" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="34" t="s">
+      <c r="E7" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="38" t="s">
         <v>19</v>
-      </c>
-      <c r="E7" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="38" t="s">
-        <v>20</v>
       </c>
       <c r="H7" s="35">
         <v>45516</v>
@@ -998,7 +1001,7 @@
       <c r="I7" s="29"/>
       <c r="J7" s="30"/>
       <c r="K7" s="31" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L7" s="32"/>
     </row>

</xml_diff>